<commit_message>
Updated graphs and data for publishing
</commit_message>
<xml_diff>
--- a/results/journal/db-stats.xlsx
+++ b/results/journal/db-stats.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">Tool</t>
   </si>
   <si>
-    <t xml:space="preserve">Time</t>
+    <t xml:space="preserve">Download time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build time</t>
   </si>
   <si>
     <t xml:space="preserve">Disk</t>
@@ -34,6 +37,9 @@
     <t xml:space="preserve">Version</t>
   </si>
   <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">DRAM</t>
   </si>
   <si>
@@ -46,10 +52,16 @@
     <t xml:space="preserve">v1.4.6</t>
   </si>
   <si>
+    <t xml:space="preserve">This is what the IT department told us</t>
+  </si>
+  <si>
     <t xml:space="preserve">InterProScan</t>
   </si>
   <si>
-    <t xml:space="preserve">~ 2:45:59.23</t>
+    <t xml:space="preserve">~ 2:34:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~ 11:32</t>
   </si>
   <si>
     <t xml:space="preserve">14GB</t>
@@ -80,6 +92,21 @@
   </si>
   <si>
     <t xml:space="preserve">v1.14.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Everything is downloaded together with bioconda install</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eggNOG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes archaea, bacteria, and virus HMMs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microbeannotator</t>
   </si>
   <si>
     <t xml:space="preserve">.</t>
@@ -89,9 +116,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="mm:ss.00"/>
+    <numFmt numFmtId="165" formatCode="hh:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="mm:ss.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -165,7 +193,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -179,6 +207,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -199,13 +231,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="44.57"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -220,66 +257,104 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
         <v>7</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G33" s="2" t="s">
-        <v>20</v>
+      <c r="H33" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>